<commit_message>
Add NSF column, error tape generator, and two-layer validator
- Add Net Servicing Fee (NSF) to 16-col tape layout: FNMA/FHLMC fixed
  at 25bps, GNMA triangular 19-69bps (median 44bps)
- build_msr_tape_errors.py: injects 22 realistic data errors (11 hard
  stops, 11 yellow lights) into a subservicer submission tape
- validate_msr_tape.py: two-layer validator that catches all injected
  errors via field-level rules (Layer 1) and cross-period comparison
  vs prior month (Layer 2); outputs Excel + Markdown reports
- Regenerated all output files with updated NSF column

Co-Authored-By: Claude Sonnet 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Recon_Capitalization_Dec2025_Jan2026.xlsx
+++ b/Recon_Capitalization_Dec2025_Jan2026.xlsx
@@ -652,54 +652,54 @@
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>MSR100079</t>
+          <t>MSR100443</t>
         </is>
       </c>
       <c r="B4" s="5" t="inlineStr">
         <is>
-          <t>90+ DPD</t>
+          <t>60 DPD</t>
         </is>
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>FHLMC</t>
+          <t>FNMA</t>
         </is>
       </c>
       <c r="D4" s="6" t="n">
-        <v>282230.01</v>
+        <v>325958.04</v>
       </c>
       <c r="E4" s="7" t="n">
-        <v>418.12</v>
+        <v>488.13</v>
       </c>
       <c r="F4" s="6" t="n">
-        <v>282648.13</v>
+        <v>326446.17</v>
       </c>
       <c r="G4" s="8" t="n">
-        <v>0.0738</v>
+        <v>0.077</v>
       </c>
       <c r="H4" s="9" t="n">
-        <v>46027</v>
+        <v>46018</v>
       </c>
       <c r="I4" s="10" t="inlineStr">
         <is>
-          <t>Deferred Interest Capitalization</t>
+          <t>Escrow Advance Capitalization</t>
         </is>
       </c>
       <c r="J4" s="11" t="inlineStr">
         <is>
-          <t>AUTH-858344</t>
+          <t>AUTH-654369</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="12" t="inlineStr">
         <is>
-          <t>MSR100530</t>
+          <t>MSR100570</t>
         </is>
       </c>
       <c r="B5" s="13" t="inlineStr">
         <is>
-          <t>60 DPD</t>
+          <t>90+ DPD</t>
         </is>
       </c>
       <c r="C5" s="12" t="inlineStr">
@@ -708,35 +708,35 @@
         </is>
       </c>
       <c r="D5" s="14" t="n">
-        <v>314377.78</v>
+        <v>439738.41</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>1060.8</v>
+        <v>399.3</v>
       </c>
       <c r="F5" s="14" t="n">
-        <v>315438.58</v>
+        <v>440137.71</v>
       </c>
       <c r="G5" s="16" t="n">
-        <v>0.0795</v>
+        <v>0.0746</v>
       </c>
       <c r="H5" s="17" t="n">
-        <v>46000</v>
+        <v>46053</v>
       </c>
       <c r="I5" s="18" t="inlineStr">
         <is>
-          <t>Escrow Advance Capitalization</t>
+          <t>Deferred Interest Capitalization</t>
         </is>
       </c>
       <c r="J5" s="19" t="inlineStr">
         <is>
-          <t>AUTH-631646</t>
+          <t>AUTH-253458</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>MSR100578</t>
+          <t>MSR100726</t>
         </is>
       </c>
       <c r="B6" s="5" t="inlineStr">
@@ -750,19 +750,19 @@
         </is>
       </c>
       <c r="D6" s="6" t="n">
-        <v>246912.29</v>
+        <v>321780.02</v>
       </c>
       <c r="E6" s="7" t="n">
-        <v>650.1799999999999</v>
+        <v>1056.05</v>
       </c>
       <c r="F6" s="6" t="n">
-        <v>247562.47</v>
+        <v>322836.07</v>
       </c>
       <c r="G6" s="8" t="n">
-        <v>0.0795</v>
+        <v>0.07630000000000001</v>
       </c>
       <c r="H6" s="9" t="n">
-        <v>46039</v>
+        <v>46025</v>
       </c>
       <c r="I6" s="10" t="inlineStr">
         <is>
@@ -771,7 +771,7 @@
       </c>
       <c r="J6" s="11" t="inlineStr">
         <is>
-          <t>AUTH-900882</t>
+          <t>AUTH-980275</t>
         </is>
       </c>
     </row>

</xml_diff>